<commit_message>
Replace old Overview.xlsx with new version (Overview 50)
</commit_message>
<xml_diff>
--- a/Overview/Overview.xlsx
+++ b/Overview/Overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\kuliah\Sem.7\Temu Kembali Informasi\UTS-tugas2\Overview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2B4C23-F7A2-45C2-B20B-C46B376BFA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6908DD0-72A0-4A89-8C16-FE8B334997CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6810" yWindow="3360" windowWidth="16485" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="154">
   <si>
     <t>No.</t>
   </si>
@@ -1276,18 +1276,237 @@
     1 (satu) buah timbangan digital warna silver.
     1 (satu) buah handphone merk Realme warna biru beserta kartu simcard dengan nomor 083849801275.</t>
   </si>
+  <si>
+    <t>544/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1 (satu) bungkus plastik klip bening yang didalamnya diduga berisikan narkotika golongan I bukan tanaman jenis shabu dengan berat bruto 1,28 (satu koma dua puluh delapan) gram yang disimpan didalam bungkus rokok Dalill warna putih</t>
+  </si>
+  <si>
+    <t>543/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1. Menyatakan Terdakwa Hasan Abdilah als Bagas Bin Alm Abdilah telah terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana, ?Permufakatan Jahat untuk melakukan tindak pidana narkotika, tanpa hak atau melawan hukum, membeli dan menerima penyerahan Narkotika Golongan I? melanggar Pasal 114 ayat (1) Jo. Pasal 132 ayat (1) UU RI No. 35 Tahun 2009 tentang Narkotika sebagaimana dakwaan Pertama Penuntut Umum;
+2. Menjatuhkan pidana penjara terhadap Terdakwa oleh karena itu dengan pidana penjara selama 5 (lima) tahun 6 (enam) bulan dan denda Rp 1.000.000,000,00 (satu milyar rupiah) dengan ketentuan apabila denda tersebut tidak dibayar diganti dengan pidana penjara selama 3 (tiga) bulan;
+3. Menetapkan masa penangkapan dan penahanan yang telah dijalani Terdakwa dikurangkan seluruhnya dari pidana yang dijatuhkan;
+4. Menetapan agar Terdakwa tetap ditahan
+5. Menetapkan barang bukti berupa:
+? 1 (satu) bungkus plastik klip bening yang didalamnya diduga berisikan narkotika golongan I bukan tanaman jenis shabu dengan berat bruto 1,28 (satu koma dua puluh delapan) gram yang disimpan didalam bungkus rokok Dalill warna putih
+Dirampas untuk dimusnahkan;
+6. Membebankan kepada terdakwa untuk membayar biaya perkara sebesar Rp 5000,00 (lima ribu rupiah).</t>
+  </si>
+  <si>
+    <t>Menyatakan Terdakwa Syaiful Arief als Gondrong Bin (alm) Ali Muchson telah terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana, ? permufakatan jahat melakukan tindak pidana narkotika, tanpa hak atau melawan hukum, membeli, dan menerima penyerahkan Narkotika Golongan I? melanggar Pasal 114 ayat (1) Jo. Pasal 132 ayat (1) UU RI No. 35 Tahun 2009 tentang Narkotika sebagaimana dakwaan Pertama Penuntut Umum;
+Menjatuhkan pidana terhadap Terdakwa oleh karena itu dengan pidana penjara selama 5 (lima) tahun 6 (enam) bulan dan denda Rp 1.000.000,000,00 (satu milyar rupiah) dengan ketentuan apabila denda tersebut tidak dibayar diganti dengan pidana penjara selama 3 (tiga) bulan;
+Menetapkan masa penangkapan dan penahanan yang telah dijalani Terdakwa dikurangkan seluruhnya dari pidana yang dijatuhkan;
+Menetapan agar Terdakwa tetap ditahan
+Menetapkan barang bukti berupa:
+1 (satu) bungkus plastik klip bening yang didalamnya diduga berisikan narkotika golongan I bukan tanaman jenis shabu dengan berat bruto 1,28 (satu koma dua puluh delapan) gram yang disimpan didalam bungkus rokok Dalill warna putih
+Dipergunakan dalam perkara Hasan Abdilah bin (Alm) Abdilah;
+Membebankan kepada terdakwa untuk membayar biaya perkara sebesar Rp 5000,00 ( lima ribu rupiah).</t>
+  </si>
+  <si>
+    <t>585/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1 (satu) bungkus plastik Klip berisikan kristal warna putih mengandung Metafetamina dengan berat netto seluruhnya 1,1440 Gram setelah dilakukan pemeriksaan menjadi berat netto seluruhnya 1,1241 Gram;
+1 (satu) buah tas selempang warna abu abu;
+1 (satu) buah timbangan warna silver;
+1 (satu) buah Handpone merk samsung Galaxy A03 warna biru dengan nomor 082114886269;</t>
+  </si>
+  <si>
+    <t>Menyatakan Terdakwa Yulianto Bin (Alm) Hadi Sucipto Jaman telah terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana secara tanpa hak menjadi perantara jual beli Narkotika Golongan ?I?, sebagaimana dakwaan Alternatif Pertama;
+Menjatuhkan pidana terhadap Terdakwa Yulianto Bin (Alm) Hadi Sucipto Jaman dengan pidana penjara selama 6 (enam) tahun dikurangi selama Terdakwa dalam tahanan dan denda sejumlah Rp1.000.000.000,00 (satu miliar rupiah) dengan ketentuan apabila denda tersebut tidak dibayar diganti dengan pidana penjara selama 3 (tiga) bulan;
+Menetapkan masa lamanya Terdakwa tersebut ditangkap dan ditahan dikurangkan seluruhnya dari Pidana yang dijatuhkan;
+Menetapkan Terdakwa tetap ditahan;
+Menyatakan Barang Bukti berupa:
+1 (satu) bungkus plastik klip berisi 10 (sepuluh) bungkus plastik masing masing berisikan 1 (satu) bungkus plastik Klip berisikan kristal warna putih mengandung Metafetamina dengan berat netto seluruhnya 1,9396 Gram setelah dilakukan pemeriksaan menjadi berat netto seluruhnya 1,9206
+1 (satu) bungkus plastik klip berisi 12 (dua belas ) bungkus plastik masing masing berisikan 1 (satu) bungkus plastik Klip berisikan kristal warna putih mengandung Metafetamina dengan berat netto seluruhnya 1,7914 Gram setelah dilakukan pemeriksaan menjadi berat netto seluruhnya 1,7652 Gram;
+1 (satu) bungkus plastik Klip berisikan kristal warna putih mengandung Metafetamina dengan berat netto seluruhnya 1,1440 Gram setelah dilakukan pemeriksaan menjadi berat netto seluruhnya 1,1241 Gram;
+1 (satu) buah tas selempang warna abu abu;
+1 (satu) buah timbangan warna silver;
+1 (satu) buah Handpone merk samsung Galaxy A03 warna biru dengan nomor 082114886269;
+Dirampas untuk dimusnahkan;
+Membebankan kepada Terdakwa untuk membayar biaya perkara sebesar Rp5.000,- (lima ribu rupiah).</t>
+  </si>
+  <si>
+    <t>545/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1. Menyatakan Terdakwa Putra Adji Pangestu Als Beler Bin Alm. Ali Muchson telah terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana, ? Permufakatan Jahat untuk melakukan tindak pidana narkotika, tanpa hak atau melawan hukum, membeli, dan menerima penyerahan Narkotika Golongan I? melanggar Pasal 114 ayat (1) Jo. Pasal 132 ayat (1) UU RI No. 35 Tahun 2009 tentang Narkotika sebagaimana dakwaan Pertama Penuntut Umum;
+2. Menjatuhkan pidana penjara terhadap Terdakwa oleh karena itu dengan pidana penjara selama 5 (lima) tahun 6 (enam) bulan dan denda Rp 1.000.000,000 (satu milyar rupiah) dengan ketentuan apabila denda tersebut tidak dibayar diganti dengan pidana penjara selama 3 (tiga) bulan;
+3. Menetapkan masa penangkapan dan penahanan yang telah dijalani Terdakwa dikurangkan seluruhnya dari pidana yang dijatuhkan;
+4. Menetapan agar Terdakwa tetap ditahan
+5. Menetapkan barang bukti berupa:
+? 1 (satu) bungkus plastik klip bening yang didalamnya diduga berisikan narkotika golongan I bukan tanaman jenis shabu dengan berat bruto 1,28 (satu koma dua puluh delapan) gram yang disimpan didalam bungkus rokok Dalill warna putih
+Dipergunakan dalam perkara Syaiful Arief als Gondrong Bin (Alm) Ali Muchson;
+6. Membebankan kepada terdakwa untuk membayar biaya perkara sebesar Rp 5000,00 ( lima ribu rupiah).</t>
+  </si>
+  <si>
+    <t>610/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1 (Satu) bungkus plastik klip bening berisi daun kering narkotika jenis ganja dengan berat brutto 4,9 ( Empat Koma Sembilan) gram didalam kotak rokok warna hitam;
+1 (Satu) bungkus plastik klip bening berisi daun kering narkotika jenis ganja dengan berat brutto 5,9 ( Lima Koma Sembilan) gram didalam wadah rantang warna abu-abu oranye ditutup kain pembungkus warna hitam.
+1 ( Satu ) buah handphone merek Xiaomi Redmi 11 Pro warna biru.</t>
+  </si>
+  <si>
+    <t>Menyatakan Terdakwa Bayu Wirawan als Bayu Bin M.Basir tidak terbukti secara sah dan menyakinkan bersalah melakukan tindak pidana sebagaimana dalam dakwaan Primair;
+Membebaskan Terdakwa Bayu Wirawan als Bayu Bin M.Basir, oleh karena itu dari dakwaan primair tersebut;
+Menyatakan Terdakwa Bayu Wirawan als Bayu Bin M.Basir, terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana ?Tanpa Hak dan melawan hukum memiliki, menyimpan dan menyediakan Narkotika Golongan I dalam bentuk tanaman? sebagaimana dalam dakwaan subsidair;
+Menjatuhkan pidana kepada Terdakwa oleh karena itu dengan pidana penjara selama 4 (EMPAT) Tahun. dan denda sejumlah Rp.1.000.000.000,00 (satu milyar rupiah), dengan ketentuan apabila denda tersebut tidak dibayar maka diganti dengan pidana penjara selama 2 (dua) bulan;
+Menetapkan masa penangkapan dan penahanan yang telah dijalani Terdakwa dikurangkan seluruhnya dari pidana yang dijatuhkan;
+Menetapkan Terdakwa tetap ditahan;
+Menetapkan barang bukti berupa:
+1 (Satu) bungkus plastik klip bening berisi daun kering narkotika jenis ganja dengan berat brutto 4,9 ( Empat Koma Sembilan) gram didalam kotak rokok warna hitam;
+1 (Satu) bungkus plastik klip bening berisi daun kering narkotika jenis ganja dengan berat brutto 5,9 ( Lima Koma Sembilan) gram didalam wadah rantang warna abu-abu oranye ditutup kain pembungkus warna hitam.
+1 ( Satu ) buah handphone merek Xiaomi Redmi 11 Pro warna biru.
+Dirampas untuk dimusnahkan .
+1 (Satu) unit sepeda motor merek VESPA dengan Nomor Polisi : D-6851-XH warna coklat.
+Dirampas untuk negara .
+Membebankan Terdakwa membayar biaya perkara sejumlah Rp.5.000,00 (lima ribu rupiah);</t>
+  </si>
+  <si>
+    <t>614/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>6 (enam) bungkus plastik klip berisikan yang mengandung Kristal Metamfetamina dengan berat netto 1,3396 gram setelah dilakukan pemeriksaan menjadi berat Netto 1,3251 gram;
+1 (satu) bungkus plastik klip berisikan yang mengandung kristal Metafetamina dengan berat netto 0,1413 gram setelah dilakukan pemeriksaan menjadi berat Netto 0,1289 gram;
+1 (satu) buah timbangan digital;
+1 (satu) buah kantong serut tali warna hitam;
+1 (satu) buah handpone merek Infinix warna putih berserta kartu perdananya dengan nomor 085770526898 ;</t>
+  </si>
+  <si>
+    <t>1. Menyatakan terdakwa ANWAR SUPRIATNA Alias IDOENK Bin (alm) TUGINO terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana ? tanpa hak atau melawan hukum memiliki, menyimpan, menguasai, atau menyediakan Narkotika Golongan I? sebagaimana dalam Dakwaan Kedua ;
+2. Menjatuhkan pidana terhadap terdakwa ANWAR SUPRIATNA Alias IDOENK Bin (alm) TUGINO, oleh karena itu dengan pidana penjara selama 5 (lima) tahun dan 6 (enam) bulan dan denda sebesar Rp 1.000.000.000,00 (satu milyar rupiah) dengan ketentuan jika denda tersebut tidak dibayarkan, maka akan diganti dengan pidana penjara selama 3 (tiga) bulan ;
+3. Menetapkan masa penangkapan dan penahanan yang telah dijalani Terdakwa dikurangkan seluruhnya dari pidana yang dijatuhkan ;
+4. Menetapkan agar terdakwa tetap ditahan ;
+5. Menyatakan Barang bukti berupa :
+- 6 (enam) bungkus plastik klip berisikan yang mengandung Kristal Metamfetamina dengan berat netto 1,3396 gram setelah dilakukan pemeriksaan menjadi berat Netto 1,3251 gram;
+- 1 (satu) bungkus plastik klip berisikan yang mengandung kristal Metafetamina dengan berat netto 0,1413 gram setelah dilakukan pemeriksaan menjadi berat Netto 0,1289 gram;
+- 1 (satu) buah timbangan digital;
+- 1 (satu) buah kantong serut tali warna hitam;
+- 1 (satu) buah handpone merek Infinix warna putih berserta kartu perdananya dengan nomor 085770526898 ;
+Dirampas untuk dimusnahkan
+6. Menghukum terdakwa membayar biaya perkara sebesar Rp.5.000,00 (lima ribu rupiah) ;</t>
+  </si>
+  <si>
+    <t>589/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1) 1 (satu) bungkus kertas kado yang didalamnya berisikan Narkotika Jenis tanaman Ganja dengan berat brutto 37,25 g (tiga puluh tujuh koma dua puluh lima gram)
+2) 1 (satu) buah Handphone merk Samsung Galaxy J7 Prime warna cream dengan nomor IMEI 1 354462089224178 Imei 2 354463089224176 dengan nomor sim card 0822883003261</t>
+  </si>
+  <si>
+    <t>1. Menyatakan terdakwa Renol Febrian Alias Renol Bin Sukardiman, telah terbukti secara sah dan meyakinan bersalah melakukan tindak pidana ?tanpa hak dan melawan hukum sebagai perantara dalam jual beli Narkotika Golongan I, sebagaimana dalam dakwaan primer;
+2. Menjatuhkan pidana terhadap Terdakwa Renol Febrian Alias Renol Bin Sukardiman oleh karena itu dengan pidana penjara selama 5 (lima) tahun dan denda sebesar Rp.1.000.000.000,00 (satu milyard rupiah) dengan ketentuan jika denda tersebut tidak dibayarkan, maka akan diganti dengan pidana penjara selama 3 (tiga) bulan ;
+3. Menetapkan masa penangkapan dan penahanan yang telah dijalani Terdakwa dikurangkan seluruhnya dari pidana yang dijatuhkan ;
+4. Menetapkan agar Terdakwa tetap ditahan;
+5. Menetapkan barang bukti berupa :
+1) 1 (satu) bungkus kertas kado yang didalamnya berisikan Narkotika Jenis tanaman Ganja dengan berat brutto 37,25 g (tiga puluh tujuh koma dua puluh lima gram)
+2) 1 (satu) buah Handphone merk Samsung Galaxy J7 Prime warna cream dengan nomor IMEI 1 354462089224178 Imei 2 354463089224176 dengan nomor sim card 0822883003261
+Dirampas untuk musnahkan.
+6. Menghukum terdakwa membayar biaya perkara sebesar Rp.5.000,00 (lima ribu rupiah) ;</t>
+  </si>
+  <si>
+    <t>621/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1 (Satu) bungkus plastik klip bening yang didalamnya berisi kristal warna putih narkotika golongan I bukan tanaman jenis shabu dengan berat brutto 3.08 (tiga koma nol delapan) gram terbungkus tisu dan masker warna putih;
+1 (satu) buah handphone merk OPPO A16 warna biru berikut simcard.</t>
+  </si>
+  <si>
+    <t>1. Menyatakan Terdakwa Dharma Tio Saputra Alias Tio Bin M. Husni telah terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana ?yang tanpa hak atau melawan hukum menawarkan untuk dijual, menjual, membeli, menerima, menjadi perantara dalam jual beli, menukar, atau menyerahkan Narkotika Golongan I? sebagaimana dakwaan Pertama Penuntut Umum ;
+2. Menjatuhkan pidana kepada Terdakwa Dharma Tio Saputra Alias Tio Bin M. Husni oleh karena itu dengan pidana penjara selama 6 ( Enam ) Tahun dan denda sebesar Rp. 1.000.000.000,00 (satu miliar rupiah) dengan ketentuan apabila denda tersebut tidak dibayar diganti dengan pidana penjara selama 4 (empat) bulan penjara.
+3. Menetapkan lamanya Terdakwa ditangkap dan ditahan dikurangkan seluruhnya dari pidana yang dijatuhkan ;
+Menetapkan agar Terdakwa tetap ditahan;
+Menetapkan barang bukti berupa :
+- 1 (Satu) bungkus plastik klip bening yang didalamnya berisi kristal warna putih narkotika golongan I bukan tanaman jenis shabu dengan berat brutto 3.08 (tiga koma nol delapan) gram terbungkus tisu dan masker warna putih;
+- 1 (satu) buah handphone merk OPPO A16 warna biru berikut simcard.
+Dirampas untuk dimusnahkan
+Menetapkan agar terdakwa membayar biaya perkara sebesar Rp. 5.000,- (lima ribu rupiah).</t>
+  </si>
+  <si>
+    <t>561/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1 (satu) buah handphone merek Oppo berwarna hitam dengan nomor 087784090568;
+1 (satu) buah handphone merek Oppo berwarna hitam dengan nomor 085819291730;</t>
+  </si>
+  <si>
+    <t>Menyatakan Terdakwa Sauwih Alias Awi Bin Raji tersebut di atas, terbukti secara sah dan meyakinkan bersalah melakukan tindak pidana ?melakukan permufakatan jahat tanpa hak atau melawan hukum menjual Narkotika Golongan I dalam bentuk bukan tanaman yang beratnya melebihi 5 gram, sebagaimana dalam dakwaan kesatu;
+Menjatuhkan pidana kepada Terdakwa oleh karena itu dengan pidana penjara selama 12 (dua belas) tahun dan pidana denda sejumlah Rp. 1.000.000.000,00 (satu milyar rupiah) dengan ketentuan apabila pidana denda tersebut tidak dibayar diganti dengan pidana penjara selama 4 (empat) bulan;
+Menetapkan barang bukti berupa :
+1 (satu) buah handphone merek Oppo berwarna hitam dengan nomor 087784090568;
+1 (satu) buah handphone merek Oppo berwarna hitam dengan nomor 085819291730;
+Dirampas untuk negara;
+Membebankan kepada Terdakwa membayar biaya perkara sejumlah Rp. 5.000,00 (lilma ribu rupiah);</t>
+  </si>
+  <si>
+    <t>599/Pid.Sus/2024/PN Bks</t>
+  </si>
+  <si>
+    <t>1 (satu) bungkus plastik ukuran besar warna bening didalamnya terdapat : 1 (satu) bungkus plastik klip didalamnya terdapat :
+1 (satu) bungkus plastik klip diberi kode A didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 10.20 berisi sabu berat brutto 10,06 (sepuluh koma nol enam) gram;
+1 (satu) bungkus plastik klip diberi kode B didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 10.20 berisi sabu berat brutto 10,02 (sepuluh koma nol dua) gram;
+1 (satu) bungkus plastik klip diberi kode C didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 10.20 berisi sabu berat brutto 9,96 (sembilan koma sembilan puluh enam) gram;
+1 (satu) bungkus plastik klip diberi kode D didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 5.15 berisi sabu berat brutto 5,16 (lima koma enam belas) gram;
+1 (satu) bungkus plastik klip diberi kode E didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 5.15 berisi sabu berat brutto 4,47 (empat koma empat puluh tujuh) gram;
+1 (satu) bungkus plastik klip diberi kode F didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 5.15 berisi sabu berat brutto 3,22 (tiga koma dua puluh dua) gram;
+Jumlah total berat brutto sabu seluruhnya 42,89 (empat puluh dua koma delapan puluh sembilan) gram;
+1 (satu) pak plastik klip merk Flexibag ukuran 5x8;
+1 (satu) pak plastik klip merk Flexibag ukuran 4x6;
+uang pecahan lima ribu rupiah yang dibuat menyerupai sendok. (Dirampas untuk negara)
+1 (satu) buah timbangan digital merk Constant;
+1 (satu) buah handphone merk Vivo No.simcard 081999188708;
+Dirampas untuk dimusnahkan</t>
+  </si>
+  <si>
+    <t>Menyatakan terdakwa AGUNG SUGIARTO bin LUKITO telah terbukti secara sah dan meyakinkan melakukan tindak pidana ?permufakatan jahat tanpa hak menawarkan untuk dijual, Narkotika Golongan I bukan tanaman yang beratnya melebihi 5 (lima) gram, dalam Surat Dakwaan Kesatu Jaksa Penuntut Umum;
+Menjatuhkan pidana terhadap terdakwa oleh karena itu dengan pidana penjara selama 10 (sepuluh ) tahun dan denda sebesar Rp 1.000.000.000,00 (satu milyar rupiah), dengan ketentuan apabila denda tidak dibayar maka diganti dengan pidana penjara selama 3 (tiga) bulan penjara;
+Menetapkan masa penangkapan dan penahanan yang telah dijalani terdakwa dikurangkan seluruhya dari pidana yang dijatuhkan;
+Menetapkan agar terdakwa tetap ditahan;
+Menetapkan barangbuktiberupa:
+1 (satu) bungkus plastik ukuran besar warna bening didalamnya terdapat : 1 (satu) bungkus plastik klip didalamnya terdapat :
+1 (satu) bungkus plastik klip diberi kode A didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 10.20 berisi sabu berat brutto 10,06 (sepuluh koma nol enam) gram;
+1 (satu) bungkus plastik klip diberi kode B didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 10.20 berisi sabu berat brutto 10,02 (sepuluh koma nol dua) gram;
+1 (satu) bungkus plastik klip diberi kode C didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 10.20 berisi sabu berat brutto 9,96 (sembilan koma sembilan puluh enam) gram;
+1 (satu) bungkus plastik klip diberi kode D didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 5.15 berisi sabu berat brutto 5,16 (lima koma enam belas) gram;
+1 (satu) bungkus plastik klip diberi kode E didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 5.15 berisi sabu berat brutto 4,47 (empat koma empat puluh tujuh) gram;
+1 (satu) bungkus plastik klip diberi kode F didalamnya terdapat 1 (satu) bungkus plastik klip bertuliskan angka 5.15 berisi sabu berat brutto 3,22 (tiga koma dua puluh dua) gram;
+Jumlah total berat brutto sabu seluruhnya 42,89 (empat puluh dua koma delapan puluh sembilan) gram;
+1 (satu) pak plastik klip merk Flexibag ukuran 5x8;
+1 (satu) pak plastik klip merk Flexibag ukuran 4x6;
+uang pecahan lima ribu rupiah yang dibuat menyerupai sendok. (Dirampas untuk negara)
+1 (satu) buah timbangan digital merk Constant;
+1 (satu) buah handphone merk Vivo No.simcard 081999188708;
+Dirampas untuk dimusnahkan
+Membebankan biaya perkara sejumlah Rp.5.000,- (lima ribu rupiah)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1325,7 +1544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1341,6 +1560,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1624,20 +1847,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.08984375" customWidth="1"/>
-    <col min="5" max="5" width="61.1796875" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="61.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1654,7 +1877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1671,7 +1894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1688,7 +1911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1705,7 +1928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1722,7 +1945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1739,7 +1962,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1756,7 +1979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1773,7 +1996,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1790,7 +2013,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1807,7 +2030,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1824,7 +2047,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1841,7 +2064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1858,7 +2081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1875,7 +2098,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1892,7 +2115,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1909,7 +2132,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1926,7 +2149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1943,7 +2166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1960,7 +2183,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1977,7 +2200,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1994,7 +2217,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2011,7 +2234,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2028,7 +2251,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2045,7 +2268,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2062,7 +2285,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2079,7 +2302,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2096,7 +2319,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2113,7 +2336,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2130,7 +2353,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2147,7 +2370,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="375" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2164,7 +2387,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2181,7 +2404,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2198,7 +2421,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2215,7 +2438,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2232,7 +2455,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2249,7 +2472,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2266,7 +2489,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2283,7 +2506,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2300,7 +2523,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2317,7 +2540,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2334,115 +2557,175 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="C42" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D42" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="375" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="C43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D43" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="C44" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="390" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="1"/>
+      <c r="B45" s="6" t="s">
+        <v>134</v>
+      </c>
       <c r="C45" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="C46" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D46" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="1"/>
+      <c r="B47" s="6" t="s">
+        <v>139</v>
+      </c>
       <c r="C47" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="375" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="C48" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D48" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="C49" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D49" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="B50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>148</v>
+      </c>
       <c r="C50" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D50" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
-      <c r="B51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="C51" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="D51" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>